<commit_message>
changed some rows in SR to " "
</commit_message>
<xml_diff>
--- a/dummydata_renamed_updated.xlsx
+++ b/dummydata_renamed_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jia yi\Desktop\dbs timesheet\Codes Python DBS\CyberSecurityCryptographyML_Hashing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56074A07-2F67-40E6-B1FA-C88DD8F4FF39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7396353D-ABD1-4A1F-AB83-244CFEE79269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIG" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="48">
   <si>
     <t>Corp CIN</t>
   </si>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1054,9 +1054,6 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
@@ -1151,9 +1148,6 @@
       </c>
       <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5">

</xml_diff>

<commit_message>
updated by continuing the codes and edit data to see the result better via codes
</commit_message>
<xml_diff>
--- a/dummydata_renamed_updated.xlsx
+++ b/dummydata_renamed_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jia yi\Desktop\dbs timesheet\Codes Python DBS\CyberSecurityCryptographyML_Hashing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7396353D-ABD1-4A1F-AB83-244CFEE79269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4184926-4CF3-4BAF-832D-1EF28C6477C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="50">
   <si>
     <t>Corp CIN</t>
   </si>
@@ -165,18 +165,31 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -213,14 +226,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,7 +983,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -980,10 +994,14 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C14" sqref="C14:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -992,7 +1010,7 @@
       <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D1" t="s">
@@ -1009,6 +1027,9 @@
       <c r="B2" t="s">
         <v>24</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D2" t="s">
         <v>36</v>
       </c>
@@ -1023,6 +1044,9 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D3" t="s">
         <v>38</v>
       </c>
@@ -1037,6 +1061,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D4" t="s">
         <v>39</v>
       </c>
@@ -1051,6 +1078,9 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" t="s">
         <v>39</v>
       </c>
@@ -1062,6 +1092,9 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D6" t="s">
         <v>39</v>
       </c>
@@ -1076,6 +1109,9 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" t="s">
         <v>38</v>
       </c>
@@ -1090,6 +1126,9 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D8" t="s">
         <v>38</v>
       </c>
@@ -1104,6 +1143,9 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1118,6 +1160,9 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1132,6 +1177,9 @@
       <c r="B11" t="s">
         <v>24</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>43</v>
       </c>
@@ -1146,6 +1194,9 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
@@ -1156,6 +1207,9 @@
       </c>
       <c r="B13" t="s">
         <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -1171,6 +1225,9 @@
       <c r="B14" t="s">
         <v>28</v>
       </c>
+      <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D14" t="s">
         <v>38</v>
       </c>
@@ -1185,6 +1242,9 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
+      <c r="C15" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1199,6 +1259,9 @@
       <c r="B16" t="s">
         <v>28</v>
       </c>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1213,6 +1276,9 @@
       <c r="B17" t="s">
         <v>31</v>
       </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1227,6 +1293,9 @@
       <c r="B18" t="s">
         <v>31</v>
       </c>
+      <c r="C18" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D18" t="s">
         <v>38</v>
       </c>
@@ -1241,6 +1310,9 @@
       <c r="B19" t="s">
         <v>31</v>
       </c>
+      <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
@@ -1249,7 +1321,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>